<commit_message>
change en_cn to en_us
</commit_message>
<xml_diff>
--- a/anqisoft.github.io.url_helper.xlsx
+++ b/anqisoft.github.io.url_helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\ecs_person\websites\anqisoft.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FD30C9-DF87-47B4-B2E3-EB41E74A52B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010828ED-85DB-40CE-9F80-2450CB8E8220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="4" activeTab="4" xr2:uid="{08EA84B6-AC3F-42FD-AF29-E2C38A5D831D}"/>
   </bookViews>
@@ -154,7 +154,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>en_cn</t>
+    <t>en_us</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -583,7 +583,7 @@
   <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.8"/>
@@ -769,7 +769,7 @@
       </c>
       <c r="E14" t="str">
         <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$1,"~lang~",OFFSET($A$2,0,B14)),"~no~",C14),"~useDice~",D14),"~zh_cn~",OFFSET($E$11,0,IF(D14="true",1,2))&amp;"，" &amp;OFFSET($A$3,C14,3)&amp;"，" &amp;OFFSET($E$2,0,B14))</f>
-        <v>&lt;a target="_blank" href="mini_poker/math.htm?lang=en_cn&amp;no=1&amp;useDice=true"&gt;&lt;en_us&gt;&lt;/en_us&gt;&lt;zh_cn&gt;带骰子，20內進位加，英文版&lt;/zh_cn&gt;&lt;zh_tw&gt;&lt;/zh_tw&gt;&lt;/a&gt;&lt;br/&gt;</v>
+        <v>&lt;a target="_blank" href="mini_poker/math.htm?lang=en_us&amp;no=1&amp;useDice=true"&gt;&lt;en_us&gt;&lt;/en_us&gt;&lt;zh_cn&gt;带骰子，20內進位加，英文版&lt;/zh_cn&gt;&lt;zh_tw&gt;&lt;/zh_tw&gt;&lt;/a&gt;&lt;br/&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -791,7 +791,7 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" ref="E15:E55" ca="1" si="4">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$1,"~lang~",OFFSET($A$2,0,B15)),"~no~",C15),"~useDice~",D15),"~zh_cn~",OFFSET($E$11,0,IF(D15="true",1,2))&amp;"，" &amp;OFFSET($A$3,C15,3)&amp;"，" &amp;OFFSET($E$2,0,B15))</f>
-        <v>&lt;a target="_blank" href="mini_poker/math.htm?lang=en_cn&amp;no=2&amp;useDice=true"&gt;&lt;en_us&gt;&lt;/en_us&gt;&lt;zh_cn&gt;带骰子，20內退位减，英文版&lt;/zh_cn&gt;&lt;zh_tw&gt;&lt;/zh_tw&gt;&lt;/a&gt;&lt;br/&gt;</v>
+        <v>&lt;a target="_blank" href="mini_poker/math.htm?lang=en_us&amp;no=2&amp;useDice=true"&gt;&lt;en_us&gt;&lt;/en_us&gt;&lt;zh_cn&gt;带骰子，20內退位减，英文版&lt;/zh_cn&gt;&lt;zh_tw&gt;&lt;/zh_tw&gt;&lt;/a&gt;&lt;br/&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -813,7 +813,7 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>&lt;a target="_blank" href="mini_poker/math.htm?lang=en_cn&amp;no=3&amp;useDice=true"&gt;&lt;en_us&gt;&lt;/en_us&gt;&lt;zh_cn&gt;带骰子，大九九乘法口訣表，英文版&lt;/zh_cn&gt;&lt;zh_tw&gt;&lt;/zh_tw&gt;&lt;/a&gt;&lt;br/&gt;</v>
+        <v>&lt;a target="_blank" href="mini_poker/math.htm?lang=en_us&amp;no=3&amp;useDice=true"&gt;&lt;en_us&gt;&lt;/en_us&gt;&lt;zh_cn&gt;带骰子，大九九乘法口訣表，英文版&lt;/zh_cn&gt;&lt;zh_tw&gt;&lt;/zh_tw&gt;&lt;/a&gt;&lt;br/&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>&lt;a target="_blank" href="mini_poker/math.htm?lang=en_cn&amp;no=1&amp;useDice=false"&gt;&lt;en_us&gt;&lt;/en_us&gt;&lt;zh_cn&gt;无骰子，20內進位加，英文版&lt;/zh_cn&gt;&lt;zh_tw&gt;&lt;/zh_tw&gt;&lt;/a&gt;&lt;br/&gt;</v>
+        <v>&lt;a target="_blank" href="mini_poker/math.htm?lang=en_us&amp;no=1&amp;useDice=false"&gt;&lt;en_us&gt;&lt;/en_us&gt;&lt;zh_cn&gt;无骰子，20內進位加，英文版&lt;/zh_cn&gt;&lt;zh_tw&gt;&lt;/zh_tw&gt;&lt;/a&gt;&lt;br/&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1253,7 +1253,7 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>&lt;a target="_blank" href="mini_poker/math.htm?lang=en_cn&amp;no=2&amp;useDice=false"&gt;&lt;en_us&gt;&lt;/en_us&gt;&lt;zh_cn&gt;无骰子，20內退位减，英文版&lt;/zh_cn&gt;&lt;zh_tw&gt;&lt;/zh_tw&gt;&lt;/a&gt;&lt;br/&gt;</v>
+        <v>&lt;a target="_blank" href="mini_poker/math.htm?lang=en_us&amp;no=2&amp;useDice=false"&gt;&lt;en_us&gt;&lt;/en_us&gt;&lt;zh_cn&gt;无骰子，20內退位减，英文版&lt;/zh_cn&gt;&lt;zh_tw&gt;&lt;/zh_tw&gt;&lt;/a&gt;&lt;br/&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1275,7 +1275,7 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>&lt;a target="_blank" href="mini_poker/math.htm?lang=en_cn&amp;no=3&amp;useDice=false"&gt;&lt;en_us&gt;&lt;/en_us&gt;&lt;zh_cn&gt;无骰子，大九九乘法口訣表，英文版&lt;/zh_cn&gt;&lt;zh_tw&gt;&lt;/zh_tw&gt;&lt;/a&gt;&lt;br/&gt;</v>
+        <v>&lt;a target="_blank" href="mini_poker/math.htm?lang=en_us&amp;no=3&amp;useDice=false"&gt;&lt;en_us&gt;&lt;/en_us&gt;&lt;zh_cn&gt;无骰子，大九九乘法口訣表，英文版&lt;/zh_cn&gt;&lt;zh_tw&gt;&lt;/zh_tw&gt;&lt;/a&gt;&lt;br/&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:5">

</xml_diff>